<commit_message>
added order file w mono cues
</commit_message>
<xml_diff>
--- a/Experiment/Orders_PILOT/PAR01_RUN01.xlsx
+++ b/Experiment/Orders_PILOT/PAR01_RUN01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24424"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VisionLab\Desktop\3DFaces\Scan Orders\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VisionLab\Desktop\3DFaces\Faces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{769B859E-365A-4287-A458-79F254774FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9EB03D5-FB4D-46BF-9F99-54F77E660A4A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948255A2-2CD3-452B-AF90-97EC33B0AFA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8964" xr2:uid="{D4DDEC22-95A9-4FBC-BC6E-676BF1E871C0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D4DDEC22-95A9-4FBC-BC6E-676BF1E871C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="62">
   <si>
     <t>Trial</t>
   </si>
@@ -211,6 +211,15 @@
   </si>
   <si>
     <t>TRUE</t>
+  </si>
+  <si>
+    <t>CoverCue.jpg</t>
+  </si>
+  <si>
+    <t>UncoverCue.jpg</t>
+  </si>
+  <si>
+    <t>CUE</t>
   </si>
 </sst>
 </file>
@@ -220,7 +229,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -582,24 +591,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{007DD0AF-B058-4617-BF46-BC504546A435}">
-  <dimension ref="A1:F211"/>
+  <dimension ref="A1:F215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="C66" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="16" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="16" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -619,7 +628,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -630,7 +639,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -650,7 +659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -670,7 +679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -690,7 +699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -710,7 +719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -730,7 +739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -750,7 +759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -770,7 +779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -790,7 +799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -810,7 +819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -830,7 +839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1</v>
       </c>
@@ -850,7 +859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1</v>
       </c>
@@ -870,7 +879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
@@ -890,7 +899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -910,7 +919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
@@ -930,7 +939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
@@ -950,7 +959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1</v>
       </c>
@@ -970,7 +979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1</v>
       </c>
@@ -990,7 +999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1010,7 +1019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1030,7 +1039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1050,7 +1059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1070,7 +1079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1090,7 +1099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1110,7 +1119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>0</v>
       </c>
@@ -1121,7 +1130,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2</v>
       </c>
@@ -1141,7 +1150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2</v>
       </c>
@@ -1161,7 +1170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2</v>
       </c>
@@ -1181,7 +1190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>2</v>
       </c>
@@ -1201,7 +1210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>2</v>
       </c>
@@ -1221,7 +1230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2</v>
       </c>
@@ -1241,7 +1250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2</v>
       </c>
@@ -1261,7 +1270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>2</v>
       </c>
@@ -1281,7 +1290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>2</v>
       </c>
@@ -1301,7 +1310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2</v>
       </c>
@@ -1321,7 +1330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2</v>
       </c>
@@ -1341,7 +1350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2</v>
       </c>
@@ -1361,7 +1370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2</v>
       </c>
@@ -1381,7 +1390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2</v>
       </c>
@@ -1401,7 +1410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>2</v>
       </c>
@@ -1421,7 +1430,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2</v>
       </c>
@@ -1441,7 +1450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>2</v>
       </c>
@@ -1461,7 +1470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>2</v>
       </c>
@@ -1481,7 +1490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>2</v>
       </c>
@@ -1501,7 +1510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2</v>
       </c>
@@ -1521,7 +1530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>2</v>
       </c>
@@ -1541,7 +1550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2</v>
       </c>
@@ -1561,7 +1570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>2</v>
       </c>
@@ -1581,7 +1590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>2</v>
       </c>
@@ -1601,7 +1610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>0</v>
       </c>
@@ -1612,7 +1621,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>3</v>
       </c>
@@ -1632,7 +1641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>3</v>
       </c>
@@ -1652,7 +1661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>3</v>
       </c>
@@ -1672,7 +1681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>3</v>
       </c>
@@ -1692,7 +1701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>3</v>
       </c>
@@ -1712,7 +1721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>3</v>
       </c>
@@ -1732,7 +1741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>3</v>
       </c>
@@ -1752,7 +1761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>3</v>
       </c>
@@ -1772,7 +1781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>3</v>
       </c>
@@ -1792,7 +1801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>3</v>
       </c>
@@ -1812,7 +1821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>3</v>
       </c>
@@ -1832,7 +1841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>3</v>
       </c>
@@ -1852,7 +1861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>3</v>
       </c>
@@ -1872,7 +1881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>3</v>
       </c>
@@ -1892,7 +1901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>3</v>
       </c>
@@ -1912,7 +1921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>3</v>
       </c>
@@ -1932,7 +1941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>3</v>
       </c>
@@ -1952,7 +1961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>3</v>
       </c>
@@ -1972,7 +1981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>3</v>
       </c>
@@ -1992,7 +2001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>3</v>
       </c>
@@ -2012,7 +2021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>3</v>
       </c>
@@ -2032,7 +2041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>3</v>
       </c>
@@ -2052,7 +2061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>3</v>
       </c>
@@ -2072,7 +2081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>3</v>
       </c>
@@ -2092,36 +2101,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>0</v>
       </c>
       <c r="B77" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C77" s="3">
+        <v>5</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F77" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>0</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C77" s="3">
+      <c r="C78" s="3">
         <v>24</v>
       </c>
-    </row>
-    <row r="78" spans="1:6">
-      <c r="A78">
-        <v>4</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C78" s="3">
-        <v>1</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="D78" s="1"/>
       <c r="E78" s="1"/>
-      <c r="F78" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6">
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>4</v>
       </c>
@@ -2132,14 +2145,14 @@
         <v>1</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E79" s="1"/>
       <c r="F79" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>4</v>
       </c>
@@ -2150,14 +2163,14 @@
         <v>1</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>4</v>
       </c>
@@ -2168,14 +2181,14 @@
         <v>1</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>4</v>
       </c>
@@ -2186,14 +2199,14 @@
         <v>1</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>4</v>
       </c>
@@ -2204,14 +2217,14 @@
         <v>1</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E83" s="1"/>
       <c r="F83" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>4</v>
       </c>
@@ -2222,14 +2235,14 @@
         <v>1</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="E84" s="1"/>
       <c r="F84" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>4</v>
       </c>
@@ -2240,14 +2253,14 @@
         <v>1</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E85" s="1"/>
       <c r="F85" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>4</v>
       </c>
@@ -2258,14 +2271,14 @@
         <v>1</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E86" s="1"/>
       <c r="F86" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>4</v>
       </c>
@@ -2276,14 +2289,14 @@
         <v>1</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E87" s="1"/>
       <c r="F87" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>4</v>
       </c>
@@ -2294,14 +2307,14 @@
         <v>1</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E88" s="1"/>
       <c r="F88" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>4</v>
       </c>
@@ -2312,14 +2325,14 @@
         <v>1</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="E89" s="1"/>
       <c r="F89" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>4</v>
       </c>
@@ -2330,14 +2343,14 @@
         <v>1</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E90" s="1"/>
       <c r="F90" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>4</v>
       </c>
@@ -2348,14 +2361,14 @@
         <v>1</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E91" s="1"/>
       <c r="F91" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>4</v>
       </c>
@@ -2366,14 +2379,14 @@
         <v>1</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E92" s="1"/>
       <c r="F92" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>4</v>
       </c>
@@ -2384,14 +2397,14 @@
         <v>1</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E93" s="1"/>
       <c r="F93" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>4</v>
       </c>
@@ -2402,14 +2415,14 @@
         <v>1</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E94" s="1"/>
       <c r="F94" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>4</v>
       </c>
@@ -2420,14 +2433,14 @@
         <v>1</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E95" s="1"/>
       <c r="F95" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>4</v>
       </c>
@@ -2438,14 +2451,14 @@
         <v>1</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E96" s="1"/>
       <c r="F96" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>4</v>
       </c>
@@ -2456,14 +2469,14 @@
         <v>1</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="E97" s="1"/>
       <c r="F97" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>4</v>
       </c>
@@ -2474,14 +2487,14 @@
         <v>1</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E98" s="1"/>
       <c r="F98" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>4</v>
       </c>
@@ -2492,14 +2505,14 @@
         <v>1</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="E99" s="1"/>
       <c r="F99" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>4</v>
       </c>
@@ -2510,14 +2523,14 @@
         <v>1</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="E100" s="1"/>
       <c r="F100" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>4</v>
       </c>
@@ -2532,61 +2545,61 @@
       </c>
       <c r="E101" s="1"/>
       <c r="F101" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102">
-        <v>0</v>
-      </c>
-      <c r="B102" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C102" s="3">
+        <v>1</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E102" s="1"/>
+      <c r="F102" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>0</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C103" s="3">
+        <v>5</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F103" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>0</v>
+      </c>
+      <c r="B104" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C102" s="3">
+      <c r="C104" s="3">
         <v>24</v>
       </c>
-    </row>
-    <row r="103" spans="1:6">
-      <c r="A103">
-        <v>5</v>
-      </c>
-      <c r="B103" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C103" s="3">
-        <v>1</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F103" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6">
-      <c r="A104">
-        <v>5</v>
-      </c>
-      <c r="B104" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C104" s="3">
-        <v>1</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E104" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F104" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6">
+      <c r="D104" s="1"/>
+      <c r="E104" s="1"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>5</v>
       </c>
@@ -2597,16 +2610,16 @@
         <v>1</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="F105" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:6">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>5</v>
       </c>
@@ -2617,16 +2630,16 @@
         <v>1</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F106" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>5</v>
       </c>
@@ -2637,16 +2650,16 @@
         <v>1</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="F107" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>5</v>
       </c>
@@ -2657,16 +2670,16 @@
         <v>1</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F108" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:6">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>5</v>
       </c>
@@ -2677,16 +2690,16 @@
         <v>1</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F109" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:6">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>5</v>
       </c>
@@ -2697,16 +2710,16 @@
         <v>1</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F110" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:6">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>5</v>
       </c>
@@ -2717,16 +2730,16 @@
         <v>1</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F111" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>5</v>
       </c>
@@ -2737,16 +2750,16 @@
         <v>1</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="F112" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>5</v>
       </c>
@@ -2757,16 +2770,16 @@
         <v>1</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F113" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:6">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>5</v>
       </c>
@@ -2777,16 +2790,16 @@
         <v>1</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="F114" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>5</v>
       </c>
@@ -2797,16 +2810,16 @@
         <v>1</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F115" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:6">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>5</v>
       </c>
@@ -2817,16 +2830,16 @@
         <v>1</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="F116" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:6">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>5</v>
       </c>
@@ -2837,16 +2850,16 @@
         <v>1</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="F117" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>5</v>
       </c>
@@ -2857,16 +2870,16 @@
         <v>1</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F118" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>5</v>
       </c>
@@ -2877,16 +2890,16 @@
         <v>1</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="F119" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>5</v>
       </c>
@@ -2897,16 +2910,16 @@
         <v>1</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="F120" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:6">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>5</v>
       </c>
@@ -2917,16 +2930,16 @@
         <v>1</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F121" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>5</v>
       </c>
@@ -2937,16 +2950,16 @@
         <v>1</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="F122" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:6">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>5</v>
       </c>
@@ -2957,16 +2970,16 @@
         <v>1</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F123" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:6">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>5</v>
       </c>
@@ -2977,16 +2990,16 @@
         <v>1</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F124" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:6">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>5</v>
       </c>
@@ -2997,16 +3010,16 @@
         <v>1</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F125" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:6">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>5</v>
       </c>
@@ -3017,67 +3030,67 @@
         <v>1</v>
       </c>
       <c r="D126" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F126" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A127">
+        <v>5</v>
+      </c>
+      <c r="B127" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C127" s="3">
+        <v>1</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F127" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A128">
+        <v>5</v>
+      </c>
+      <c r="B128" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C128" s="3">
+        <v>1</v>
+      </c>
+      <c r="D128" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E126" s="1" t="s">
+      <c r="E128" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F126" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6">
-      <c r="A127">
-        <v>0</v>
-      </c>
-      <c r="B127" s="1" t="s">
+      <c r="F128" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A129">
+        <v>0</v>
+      </c>
+      <c r="B129" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C127" s="3">
+      <c r="C129" s="3">
         <v>24</v>
       </c>
     </row>
-    <row r="128" spans="1:6">
-      <c r="A128">
-        <v>6</v>
-      </c>
-      <c r="B128" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C128" s="3">
-        <v>1</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E128" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F128" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6">
-      <c r="A129">
-        <v>6</v>
-      </c>
-      <c r="B129" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C129" s="3">
-        <v>1</v>
-      </c>
-      <c r="D129" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E129" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F129" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>6</v>
       </c>
@@ -3088,16 +3101,16 @@
         <v>1</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="F130" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:6">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>6</v>
       </c>
@@ -3108,16 +3121,16 @@
         <v>1</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="F131" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:6">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>6</v>
       </c>
@@ -3128,16 +3141,16 @@
         <v>1</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F132" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:6">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>6</v>
       </c>
@@ -3148,16 +3161,16 @@
         <v>1</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F133" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:6">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>6</v>
       </c>
@@ -3168,16 +3181,16 @@
         <v>1</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F134" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:6">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>6</v>
       </c>
@@ -3188,16 +3201,16 @@
         <v>1</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F135" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:6">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>6</v>
       </c>
@@ -3208,16 +3221,16 @@
         <v>1</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F136" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:6">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>6</v>
       </c>
@@ -3228,16 +3241,16 @@
         <v>1</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="F137" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:6">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>6</v>
       </c>
@@ -3248,16 +3261,16 @@
         <v>1</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F138" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:6">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>6</v>
       </c>
@@ -3268,16 +3281,16 @@
         <v>1</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="F139" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:6">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>6</v>
       </c>
@@ -3288,16 +3301,16 @@
         <v>1</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F140" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:6">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>6</v>
       </c>
@@ -3308,16 +3321,16 @@
         <v>1</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F141" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:6">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>6</v>
       </c>
@@ -3328,16 +3341,16 @@
         <v>1</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F142" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>6</v>
       </c>
@@ -3348,16 +3361,16 @@
         <v>1</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F143" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:6">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>6</v>
       </c>
@@ -3368,16 +3381,16 @@
         <v>1</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F144" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>6</v>
       </c>
@@ -3388,16 +3401,16 @@
         <v>1</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="F145" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:6">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>6</v>
       </c>
@@ -3408,16 +3421,16 @@
         <v>1</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="F146" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:6">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>6</v>
       </c>
@@ -3428,16 +3441,16 @@
         <v>1</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F147" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:6">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>6</v>
       </c>
@@ -3448,16 +3461,16 @@
         <v>1</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F148" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:6">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>6</v>
       </c>
@@ -3468,16 +3481,16 @@
         <v>1</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F149" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:6">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>6</v>
       </c>
@@ -3488,16 +3501,16 @@
         <v>1</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F150" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:6">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>6</v>
       </c>
@@ -3508,99 +3521,107 @@
         <v>1</v>
       </c>
       <c r="D151" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F151" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A152">
+        <v>6</v>
+      </c>
+      <c r="B152" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C152" s="3">
+        <v>1</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E152" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F152" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A153">
+        <v>6</v>
+      </c>
+      <c r="B153" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C153" s="3">
+        <v>1</v>
+      </c>
+      <c r="D153" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E151" s="1" t="s">
+      <c r="E153" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F151" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6">
-      <c r="A152">
-        <v>0</v>
-      </c>
-      <c r="B152" s="1" t="s">
+      <c r="F153" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A154">
+        <v>0</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C154" s="3">
+        <v>5</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F154" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A155">
+        <v>0</v>
+      </c>
+      <c r="B155" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C152" s="3">
+      <c r="C155" s="3">
         <v>24</v>
       </c>
-    </row>
-    <row r="153" spans="1:6">
-      <c r="A153">
-        <v>7</v>
-      </c>
-      <c r="B153" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C153" s="3">
-        <v>1</v>
-      </c>
-      <c r="D153" s="1" t="s">
+      <c r="D155" s="1"/>
+      <c r="E155" s="1"/>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A156">
+        <v>7</v>
+      </c>
+      <c r="B156" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C156" s="3">
+        <v>1</v>
+      </c>
+      <c r="D156" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="E153" s="1"/>
-      <c r="F153" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6">
-      <c r="A154">
-        <v>7</v>
-      </c>
-      <c r="B154" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C154" s="3">
-        <v>1</v>
-      </c>
-      <c r="D154" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E154" s="1"/>
-      <c r="F154" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6">
-      <c r="A155">
-        <v>7</v>
-      </c>
-      <c r="B155" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C155" s="3">
-        <v>1</v>
-      </c>
-      <c r="D155" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E155" s="1"/>
-      <c r="F155" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6">
-      <c r="A156">
-        <v>7</v>
-      </c>
-      <c r="B156" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C156" s="3">
-        <v>1</v>
-      </c>
-      <c r="D156" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="E156" s="1"/>
       <c r="F156" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:6">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>7</v>
       </c>
@@ -3611,14 +3632,14 @@
         <v>1</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E157" s="1"/>
       <c r="F157" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:6">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>7</v>
       </c>
@@ -3629,14 +3650,14 @@
         <v>1</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E158" s="1"/>
       <c r="F158" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:6">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>7</v>
       </c>
@@ -3647,14 +3668,14 @@
         <v>1</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E159" s="1"/>
       <c r="F159" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:6">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>7</v>
       </c>
@@ -3665,14 +3686,14 @@
         <v>1</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="E160" s="1"/>
       <c r="F160" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:6">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>7</v>
       </c>
@@ -3683,14 +3704,14 @@
         <v>1</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E161" s="1"/>
       <c r="F161" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:6">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>7</v>
       </c>
@@ -3701,14 +3722,14 @@
         <v>1</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E162" s="1"/>
       <c r="F162" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:6">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>7</v>
       </c>
@@ -3719,14 +3740,14 @@
         <v>1</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="E163" s="1"/>
       <c r="F163" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:6">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>7</v>
       </c>
@@ -3737,14 +3758,14 @@
         <v>1</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E164" s="1"/>
       <c r="F164" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:6">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>7</v>
       </c>
@@ -3755,14 +3776,14 @@
         <v>1</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E165" s="1"/>
       <c r="F165" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>7</v>
       </c>
@@ -3773,14 +3794,14 @@
         <v>1</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="E166" s="1"/>
       <c r="F166" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:6">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>7</v>
       </c>
@@ -3791,14 +3812,14 @@
         <v>1</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="E167" s="1"/>
       <c r="F167" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:6">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>7</v>
       </c>
@@ -3809,14 +3830,14 @@
         <v>1</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E168" s="1"/>
       <c r="F168" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>7</v>
       </c>
@@ -3827,14 +3848,14 @@
         <v>1</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E169" s="1"/>
       <c r="F169" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:6">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>7</v>
       </c>
@@ -3845,14 +3866,14 @@
         <v>1</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E170" s="1"/>
       <c r="F170" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:6">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>7</v>
       </c>
@@ -3863,14 +3884,14 @@
         <v>1</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E171" s="1"/>
       <c r="F171" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:6">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>7</v>
       </c>
@@ -3881,14 +3902,14 @@
         <v>1</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E172" s="1"/>
       <c r="F172" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:6">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>7</v>
       </c>
@@ -3899,14 +3920,14 @@
         <v>1</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E173" s="1"/>
       <c r="F173" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:6">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>7</v>
       </c>
@@ -3917,14 +3938,14 @@
         <v>1</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E174" s="1"/>
       <c r="F174" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:6">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>7</v>
       </c>
@@ -3935,14 +3956,14 @@
         <v>1</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E175" s="1"/>
       <c r="F175" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:6">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>7</v>
       </c>
@@ -3953,105 +3974,101 @@
         <v>1</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E176" s="1"/>
       <c r="F176" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:6">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A177">
-        <v>0</v>
-      </c>
-      <c r="B177" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B177" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C177" s="3">
+        <v>1</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E177" s="1"/>
+      <c r="F177" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A178">
+        <v>7</v>
+      </c>
+      <c r="B178" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C178" s="3">
+        <v>1</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E178" s="1"/>
+      <c r="F178" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A179">
+        <v>7</v>
+      </c>
+      <c r="B179" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C179" s="3">
+        <v>1</v>
+      </c>
+      <c r="D179" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E179" s="1"/>
+      <c r="F179" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A180">
+        <v>0</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C180" s="3">
+        <v>5</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E180" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F180" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A181">
+        <v>0</v>
+      </c>
+      <c r="B181" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C177" s="3">
+      <c r="C181" s="3">
         <v>24</v>
       </c>
-    </row>
-    <row r="178" spans="1:6">
-      <c r="A178">
-        <v>8</v>
-      </c>
-      <c r="B178" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C178" s="3">
-        <v>1</v>
-      </c>
-      <c r="D178" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E178" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F178" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6">
-      <c r="A179">
-        <v>8</v>
-      </c>
-      <c r="B179" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C179" s="3">
-        <v>1</v>
-      </c>
-      <c r="D179" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E179" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F179" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6">
-      <c r="A180">
-        <v>8</v>
-      </c>
-      <c r="B180" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C180" s="3">
-        <v>1</v>
-      </c>
-      <c r="D180" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E180" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F180" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6">
-      <c r="A181">
-        <v>8</v>
-      </c>
-      <c r="B181" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C181" s="3">
-        <v>1</v>
-      </c>
-      <c r="D181" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E181" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F181" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6">
+      <c r="D181" s="1"/>
+      <c r="E181" s="1"/>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>8</v>
       </c>
@@ -4062,16 +4079,16 @@
         <v>1</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F182" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="183" spans="1:6">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>8</v>
       </c>
@@ -4082,16 +4099,16 @@
         <v>1</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F183" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="184" spans="1:6">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>8</v>
       </c>
@@ -4102,16 +4119,16 @@
         <v>1</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F184" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="185" spans="1:6">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>8</v>
       </c>
@@ -4122,16 +4139,16 @@
         <v>1</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="F185" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="186" spans="1:6">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>8</v>
       </c>
@@ -4142,16 +4159,16 @@
         <v>1</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="F186" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="187" spans="1:6">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>8</v>
       </c>
@@ -4162,16 +4179,16 @@
         <v>1</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="F187" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="188" spans="1:6">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>8</v>
       </c>
@@ -4182,16 +4199,16 @@
         <v>1</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="F188" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="189" spans="1:6">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>8</v>
       </c>
@@ -4202,16 +4219,16 @@
         <v>1</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="F189" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="190" spans="1:6">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>8</v>
       </c>
@@ -4222,16 +4239,16 @@
         <v>1</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F190" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="191" spans="1:6">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>8</v>
       </c>
@@ -4242,16 +4259,16 @@
         <v>1</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F191" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="192" spans="1:6">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>8</v>
       </c>
@@ -4262,16 +4279,16 @@
         <v>1</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="F192" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="193" spans="1:6">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>8</v>
       </c>
@@ -4282,16 +4299,16 @@
         <v>1</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E193" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F193" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="194" spans="1:6">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>8</v>
       </c>
@@ -4302,16 +4319,16 @@
         <v>1</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="F194" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="195" spans="1:6">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>8</v>
       </c>
@@ -4322,16 +4339,16 @@
         <v>1</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="F195" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="196" spans="1:6">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>8</v>
       </c>
@@ -4342,16 +4359,16 @@
         <v>1</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="F196" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="197" spans="1:6" ht="15">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>8</v>
       </c>
@@ -4362,16 +4379,16 @@
         <v>1</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="F197" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="198" spans="1:6">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>8</v>
       </c>
@@ -4382,16 +4399,16 @@
         <v>1</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F198" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="199" spans="1:6">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>8</v>
       </c>
@@ -4402,16 +4419,16 @@
         <v>1</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F199" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="200" spans="1:6">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>8</v>
       </c>
@@ -4422,16 +4439,16 @@
         <v>1</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F200" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="201" spans="1:6">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>8</v>
       </c>
@@ -4442,37 +4459,117 @@
         <v>1</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="F201" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="202" spans="1:6">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A202">
-        <v>0</v>
-      </c>
-      <c r="B202" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B202" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C202" s="3">
+        <v>1</v>
+      </c>
+      <c r="D202" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E202" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F202" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A203">
+        <v>8</v>
+      </c>
+      <c r="B203" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C203" s="3">
+        <v>1</v>
+      </c>
+      <c r="D203" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E203" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F203" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A204">
+        <v>8</v>
+      </c>
+      <c r="B204" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C204" s="3">
+        <v>1</v>
+      </c>
+      <c r="D204" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E204" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F204" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A205">
+        <v>8</v>
+      </c>
+      <c r="B205" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C205" s="3">
+        <v>1</v>
+      </c>
+      <c r="D205" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E205" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F205" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A206">
+        <v>0</v>
+      </c>
+      <c r="B206" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C202" s="3">
+      <c r="C206" s="3">
         <v>16</v>
       </c>
     </row>
-    <row r="204" spans="1:6">
-      <c r="C204" s="5"/>
-    </row>
-    <row r="205" spans="1:6">
-      <c r="C205" s="6"/>
-    </row>
-    <row r="206" spans="1:6">
-      <c r="C206" s="7"/>
-    </row>
-    <row r="211" spans="5:5">
-      <c r="E211" s="7"/>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C208" s="5"/>
+    </row>
+    <row r="209" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C209" s="6"/>
+    </row>
+    <row r="210" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C210" s="7"/>
+    </row>
+    <row r="215" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E215" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed ord 1 baseline timing
</commit_message>
<xml_diff>
--- a/Experiment/Orders_PILOT/PAR01_RUN01.xlsx
+++ b/Experiment/Orders_PILOT/PAR01_RUN01.xlsx
@@ -592,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G78" sqref="G78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,7 +635,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="3">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1126,7 +1126,7 @@
         <v>6</v>
       </c>
       <c r="C27" s="3">
-        <v>2</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1617,7 +1617,7 @@
         <v>6</v>
       </c>
       <c r="C52" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -2128,7 +2128,7 @@
         <v>6</v>
       </c>
       <c r="C78" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>

</xml_diff>